<commit_message>
found mistakes were fixed
</commit_message>
<xml_diff>
--- a/Lab2/excel_files/lintroller_test.xlsx
+++ b/Lab2/excel_files/lintroller_test.xlsx
@@ -20,12 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
   <si>
     <t xml:space="preserve">bool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lintroller_100</t>
   </si>
   <si>
     <t xml:space="preserve">lintroller_81</t>
@@ -186,10 +189,10 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P2" activeCellId="0" sqref="P2"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -203,7 +206,7 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="n">
+      <c r="B2" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -236,7 +239,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -244,7 +247,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -276,7 +279,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -284,7 +287,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -316,7 +319,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -324,7 +327,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -332,7 +335,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -340,7 +343,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -352,8 +355,12 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
+      <c r="A21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
added addition instances for training and test sets
</commit_message>
<xml_diff>
--- a/Lab2/excel_files/lintroller_test.xlsx
+++ b/Lab2/excel_files/lintroller_test.xlsx
@@ -10,7 +10,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -86,6 +86,51 @@
   </si>
   <si>
     <t xml:space="preserve">lintroller_99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lintroller_131</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lintroller_132</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lintroller_133</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lintroller_134</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lintroller_135</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lintroller_136</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lintroller_137</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lintroller_138</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lintroller_139</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lintroller_140</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lintroller_141</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lintroller_142</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lintroller_143</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lintroller_144</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lintroller_145</t>
   </si>
 </sst>
 </file>
@@ -186,15 +231,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -202,7 +247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -210,7 +255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -218,7 +263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -226,7 +271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -234,7 +279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -242,7 +287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -250,7 +295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -258,7 +303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -266,7 +311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -274,7 +319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -282,7 +327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -290,7 +335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -298,7 +343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -306,7 +351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
@@ -314,7 +359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -322,7 +367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -330,7 +375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
@@ -338,7 +383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -346,7 +391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
@@ -354,11 +399,131 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B21" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" s="0" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>